<commit_message>
deleted:    hardware/v2/4c/myocap4c_v2_gbr.ZIP 	deleted:    hardware/v2/4c/myocap4c_v2_proteus.pdsprj 	deleted:    hardware/v2/4c/myocap4c_v2_schematic.PDF 	modified:   hardware/v2/tiva shield/tivashield_v2_bom.xlsx 	modified:   hardware/v2/tiva shield/tivashield_v2_gbr.ZIP 	modified:   hardware/v2/tiva shield/tivashield_v2_proteus.pdsprj 	deleted:    hardware/v2/tiva shield/tivashield_v2_schematic.PDF
</commit_message>
<xml_diff>
--- a/hardware/v2/tiva shield/tivashield_v2_bom.xlsx
+++ b/hardware/v2/tiva shield/tivashield_v2_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Template" sheetId="1" state="visible" r:id="rId2"/>
@@ -64,10 +64,10 @@
     <t xml:space="preserve">REG</t>
   </si>
   <si>
-    <t xml:space="preserve">LM1117T-5.0/NOPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=LM1117T-5.0%2FNOPB-ND</t>
+    <t xml:space="preserve">LM7805CT/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/texas-instruments/LM7805CT-NOPB/296-47192-ND/3901929</t>
   </si>
   <si>
     <t xml:space="preserve">POWER</t>
@@ -240,19 +240,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="87.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.437037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.3925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.97777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="89.5666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,29 +367,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPTC061LFBN-RC/S7004-ND/810145"/>
     <hyperlink ref="D3" r:id="rId2" display="https://www.digikey.co.il/product-detail/en/amphenol-icc-fci/68002-404HLF/609-3305-ND/1878460"/>
     <hyperlink ref="D4" r:id="rId3" display="https://www.digikey.co.il/product-detail/en/amphenol-icc-fci/67996-420HLF/609-3221-ND/1878553"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://www.digikey.com/products/en?keywords=LM1117T-5.0%2FNOPB-ND"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://www.digikey.com/product-detail/en/texas-instruments/LM7805CT-NOPB/296-47192-ND/3901929"/>
     <hyperlink ref="D6" r:id="rId5" display="https://www.digikey.com/products/en?mpart=22-04-1031&amp;v=23"/>
     <hyperlink ref="D7" r:id="rId6" display="https://www.digikey.com/products/en?mpart=22-04-1031&amp;v=24"/>
     <hyperlink ref="D8" r:id="rId7" display="https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/CF14JT1K00/CF14JT1K00TR-ND/1741314"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>